<commit_message>
hand and hide labels
</commit_message>
<xml_diff>
--- a/тесты.xlsx
+++ b/тесты.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\aia_git\ai_annotator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B1FEF3-76F5-4CAC-9900-E647398C312E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1FE505-1404-447A-B405-0D6841FAE064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
   <si>
     <t>Создать полигон</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Обнаружение объектов сканированием</t>
+  </si>
+  <si>
+    <t>Корректное добавление объектов в случае ухода с детектируемого изображения</t>
   </si>
 </sst>
 </file>
@@ -616,10 +619,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:B128"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,27 +1014,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+    <row r="65" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B67" s="3"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>5</v>
@@ -1039,7 +1042,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>5</v>
@@ -1047,7 +1050,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>5</v>
@@ -1055,37 +1058,37 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
+      <c r="B72" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="4" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B75" s="3"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>5</v>
@@ -1093,7 +1096,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>5</v>
@@ -1101,7 +1104,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>5</v>
@@ -1109,15 +1112,19 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B79" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
+      <c r="B80" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
@@ -1127,23 +1134,19 @@
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
     </row>
-    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="4" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B84" s="3"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>5</v>
@@ -1151,15 +1154,19 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
+      <c r="B87" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
@@ -1169,23 +1176,19 @@
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
     </row>
-    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+    </row>
+    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B91" s="3"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>5</v>
@@ -1193,7 +1196,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>5</v>
@@ -1201,7 +1204,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>5</v>
@@ -1209,7 +1212,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>5</v>
@@ -1217,37 +1220,41 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B96" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
+      <c r="B97" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
     </row>
-    <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="4" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+    </row>
+    <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="3" t="s">
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B100" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
+      <c r="B101" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
@@ -1356,6 +1363,10 @@
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="3"/>
+      <c r="B129" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>